<commit_message>
Update - Revue 2 - Planning réel sur 200h - Joris HURTEL
</commit_message>
<xml_diff>
--- a/Documentation/Joris HURTEL/Revue 2 - Planning réel sur 200h - Joris HURTEL.xlsx
+++ b/Documentation/Joris HURTEL/Revue 2 - Planning réel sur 200h - Joris HURTEL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joris\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joris\Desktop\Revue 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DDF32A-A3E0-4E42-A894-D0CE340D9223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0DA450-ABCC-4EA3-B78B-C9AB5BA20B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -247,12 +247,6 @@
     <t>Correction des livrables (9h)</t>
   </si>
   <si>
-    <t>REVUE 2 - COMPREHENSION, RECHERCHES ET REALISATION SUR MAQUETTE DU PROJET (50h30min)</t>
-  </si>
-  <si>
-    <t>REVUE 3 - REALISATION DU PROJET SUR LE TERRAIN (91h30min)</t>
-  </si>
-  <si>
     <t>REVUE 2 - Compréhension et recherches sur le projet et maquettage (50h30min)</t>
   </si>
   <si>
@@ -266,6 +260,12 @@
   </si>
   <si>
     <t>xx/xx/2024</t>
+  </si>
+  <si>
+    <t>REVUE 2 - COMPREHENSION, RECHERCHES ET REALISATION SUR MAQUETTE DU PROJET (50h)</t>
+  </si>
+  <si>
+    <t>REVUE 3 - REALISATION DU PROJET SUR LE TERRAIN (92h)</t>
   </si>
 </sst>
 </file>
@@ -1077,25 +1077,57 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1109,59 +1141,27 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,8 +1483,8 @@
   </sheetPr>
   <dimension ref="A1:CJ80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BP46" sqref="BP46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ49" sqref="AJ49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1592,40 +1592,40 @@
     </row>
     <row r="2" spans="1:88" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="119"/>
-      <c r="R2" s="119"/>
-      <c r="S2" s="119"/>
-      <c r="T2" s="119"/>
-      <c r="U2" s="119"/>
-      <c r="V2" s="119"/>
-      <c r="W2" s="119"/>
-      <c r="X2" s="119"/>
-      <c r="Y2" s="119"/>
-      <c r="Z2" s="119"/>
-      <c r="AA2" s="119"/>
-      <c r="AB2" s="119"/>
-      <c r="AC2" s="119"/>
-      <c r="AD2" s="119"/>
-      <c r="AE2" s="119"/>
-      <c r="AF2" s="119"/>
-      <c r="AG2" s="119"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="131"/>
+      <c r="V2" s="131"/>
+      <c r="W2" s="131"/>
+      <c r="X2" s="131"/>
+      <c r="Y2" s="131"/>
+      <c r="Z2" s="131"/>
+      <c r="AA2" s="131"/>
+      <c r="AB2" s="131"/>
+      <c r="AC2" s="131"/>
+      <c r="AD2" s="131"/>
+      <c r="AE2" s="131"/>
+      <c r="AF2" s="131"/>
+      <c r="AG2" s="131"/>
       <c r="AH2" s="13"/>
       <c r="AI2" s="13"/>
       <c r="AJ2" s="13"/>
@@ -1774,41 +1774,41 @@
     </row>
     <row r="4" spans="1:88" ht="21.75" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1"/>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="123" t="s">
+      <c r="C4" s="135"/>
+      <c r="D4" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="135"/>
       <c r="H4" s="18"/>
-      <c r="I4" s="122" t="s">
+      <c r="I4" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="124" t="s">
+      <c r="J4" s="135"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="135"/>
+      <c r="M4" s="135"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="112"/>
-      <c r="Y4" s="112"/>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
+      <c r="Q4" s="135"/>
+      <c r="R4" s="135"/>
+      <c r="S4" s="135"/>
+      <c r="T4" s="135"/>
+      <c r="U4" s="135"/>
+      <c r="V4" s="135"/>
+      <c r="W4" s="135"/>
+      <c r="X4" s="135"/>
+      <c r="Y4" s="135"/>
+      <c r="Z4" s="135"/>
+      <c r="AA4" s="135"/>
+      <c r="AB4" s="135"/>
       <c r="AC4" s="19"/>
       <c r="AD4" s="10"/>
       <c r="AE4" s="10"/>
@@ -1872,10 +1872,10 @@
     </row>
     <row r="5" spans="1:88" ht="51" x14ac:dyDescent="0.6">
       <c r="A5" s="1"/>
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="112"/>
+      <c r="C5" s="135"/>
       <c r="D5" s="20" t="s">
         <v>5</v>
       </c>
@@ -1883,29 +1883,29 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="122" t="s">
+      <c r="I5" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="111">
+      <c r="J5" s="135"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="135"/>
+      <c r="M5" s="135"/>
+      <c r="N5" s="135"/>
+      <c r="O5" s="135"/>
+      <c r="P5" s="141">
         <v>45306</v>
       </c>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="112"/>
-      <c r="X5" s="112"/>
-      <c r="Y5" s="112"/>
-      <c r="Z5" s="112"/>
-      <c r="AA5" s="112"/>
+      <c r="Q5" s="135"/>
+      <c r="R5" s="135"/>
+      <c r="S5" s="135"/>
+      <c r="T5" s="135"/>
+      <c r="U5" s="135"/>
+      <c r="V5" s="135"/>
+      <c r="W5" s="135"/>
+      <c r="X5" s="135"/>
+      <c r="Y5" s="135"/>
+      <c r="Z5" s="135"/>
+      <c r="AA5" s="135"/>
       <c r="AB5" s="22"/>
       <c r="AC5" s="19"/>
       <c r="AD5" s="1"/>
@@ -2150,245 +2150,245 @@
     </row>
     <row r="8" spans="1:88" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="109" t="s">
+      <c r="D8" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="109" t="s">
+      <c r="E8" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="109" t="s">
+      <c r="F8" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="109" t="s">
+      <c r="G8" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="109" t="s">
+      <c r="H8" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="113" t="s">
+      <c r="I8" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="110"/>
-      <c r="S8" s="110"/>
-      <c r="T8" s="110"/>
-      <c r="U8" s="110"/>
-      <c r="V8" s="110"/>
-      <c r="W8" s="110"/>
-      <c r="X8" s="110"/>
-      <c r="Y8" s="110"/>
-      <c r="Z8" s="110"/>
-      <c r="AA8" s="110"/>
-      <c r="AB8" s="110"/>
-      <c r="AC8" s="110"/>
-      <c r="AD8" s="110"/>
-      <c r="AE8" s="110"/>
-      <c r="AF8" s="110"/>
-      <c r="AG8" s="110"/>
-      <c r="AH8" s="114" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI8" s="139"/>
-      <c r="AJ8" s="139"/>
-      <c r="AK8" s="139"/>
-      <c r="AL8" s="139"/>
-      <c r="AM8" s="139"/>
-      <c r="AN8" s="139"/>
-      <c r="AO8" s="139"/>
-      <c r="AP8" s="139"/>
-      <c r="AQ8" s="139"/>
-      <c r="AR8" s="139"/>
-      <c r="AS8" s="139"/>
-      <c r="AT8" s="139"/>
-      <c r="AU8" s="139"/>
-      <c r="AV8" s="139"/>
-      <c r="AW8" s="139"/>
-      <c r="AX8" s="139"/>
-      <c r="AY8" s="139"/>
-      <c r="AZ8" s="139"/>
-      <c r="BA8" s="139"/>
-      <c r="BB8" s="139"/>
-      <c r="BC8" s="139"/>
-      <c r="BD8" s="139"/>
-      <c r="BE8" s="139"/>
-      <c r="BF8" s="139"/>
-      <c r="BG8" s="139"/>
-      <c r="BH8" s="139"/>
-      <c r="BI8" s="139"/>
-      <c r="BJ8" s="139"/>
-      <c r="BK8" s="139"/>
-      <c r="BL8" s="139"/>
-      <c r="BM8" s="139"/>
-      <c r="BN8" s="139"/>
-      <c r="BO8" s="139"/>
-      <c r="BP8" s="139"/>
-      <c r="BQ8" s="116" t="s">
-        <v>72</v>
-      </c>
-      <c r="BR8" s="115"/>
-      <c r="BS8" s="115"/>
-      <c r="BT8" s="115"/>
-      <c r="BU8" s="115"/>
-      <c r="BV8" s="115"/>
-      <c r="BW8" s="115"/>
-      <c r="BX8" s="115"/>
-      <c r="BY8" s="115"/>
-      <c r="BZ8" s="115"/>
-      <c r="CA8" s="115"/>
-      <c r="CB8" s="115"/>
-      <c r="CC8" s="115"/>
-      <c r="CD8" s="115"/>
-      <c r="CE8" s="115"/>
-      <c r="CF8" s="115"/>
-      <c r="CG8" s="115"/>
-      <c r="CH8" s="115"/>
-      <c r="CI8" s="115"/>
-      <c r="CJ8" s="117"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="113"/>
+      <c r="Y8" s="113"/>
+      <c r="Z8" s="113"/>
+      <c r="AA8" s="113"/>
+      <c r="AB8" s="113"/>
+      <c r="AC8" s="113"/>
+      <c r="AD8" s="113"/>
+      <c r="AE8" s="113"/>
+      <c r="AF8" s="113"/>
+      <c r="AG8" s="113"/>
+      <c r="AH8" s="139" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI8" s="140"/>
+      <c r="AJ8" s="140"/>
+      <c r="AK8" s="140"/>
+      <c r="AL8" s="140"/>
+      <c r="AM8" s="140"/>
+      <c r="AN8" s="140"/>
+      <c r="AO8" s="140"/>
+      <c r="AP8" s="140"/>
+      <c r="AQ8" s="140"/>
+      <c r="AR8" s="140"/>
+      <c r="AS8" s="140"/>
+      <c r="AT8" s="140"/>
+      <c r="AU8" s="140"/>
+      <c r="AV8" s="140"/>
+      <c r="AW8" s="140"/>
+      <c r="AX8" s="140"/>
+      <c r="AY8" s="140"/>
+      <c r="AZ8" s="140"/>
+      <c r="BA8" s="140"/>
+      <c r="BB8" s="140"/>
+      <c r="BC8" s="140"/>
+      <c r="BD8" s="140"/>
+      <c r="BE8" s="140"/>
+      <c r="BF8" s="140"/>
+      <c r="BG8" s="140"/>
+      <c r="BH8" s="140"/>
+      <c r="BI8" s="140"/>
+      <c r="BJ8" s="140"/>
+      <c r="BK8" s="140"/>
+      <c r="BL8" s="140"/>
+      <c r="BM8" s="140"/>
+      <c r="BN8" s="140"/>
+      <c r="BO8" s="140"/>
+      <c r="BP8" s="140"/>
+      <c r="BQ8" s="129" t="s">
+        <v>77</v>
+      </c>
+      <c r="BR8" s="127"/>
+      <c r="BS8" s="127"/>
+      <c r="BT8" s="127"/>
+      <c r="BU8" s="127"/>
+      <c r="BV8" s="127"/>
+      <c r="BW8" s="127"/>
+      <c r="BX8" s="127"/>
+      <c r="BY8" s="127"/>
+      <c r="BZ8" s="127"/>
+      <c r="CA8" s="127"/>
+      <c r="CB8" s="127"/>
+      <c r="CC8" s="127"/>
+      <c r="CD8" s="127"/>
+      <c r="CE8" s="127"/>
+      <c r="CF8" s="127"/>
+      <c r="CG8" s="127"/>
+      <c r="CH8" s="127"/>
+      <c r="CI8" s="127"/>
+      <c r="CJ8" s="128"/>
     </row>
     <row r="9" spans="1:88" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="110"/>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="130" t="s">
+      <c r="B9" s="113"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="126"/>
-      <c r="K9" s="126"/>
-      <c r="L9" s="126"/>
-      <c r="M9" s="127"/>
-      <c r="N9" s="131" t="s">
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="O9" s="126"/>
-      <c r="P9" s="126"/>
-      <c r="Q9" s="126"/>
-      <c r="R9" s="127"/>
-      <c r="S9" s="131" t="s">
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="121"/>
+      <c r="R9" s="122"/>
+      <c r="S9" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="126"/>
-      <c r="U9" s="126"/>
-      <c r="V9" s="126"/>
-      <c r="W9" s="127"/>
-      <c r="X9" s="131" t="s">
+      <c r="T9" s="121"/>
+      <c r="U9" s="121"/>
+      <c r="V9" s="121"/>
+      <c r="W9" s="122"/>
+      <c r="X9" s="124" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="126"/>
-      <c r="Z9" s="126"/>
-      <c r="AA9" s="126"/>
-      <c r="AB9" s="127"/>
-      <c r="AC9" s="131" t="s">
+      <c r="Y9" s="121"/>
+      <c r="Z9" s="121"/>
+      <c r="AA9" s="121"/>
+      <c r="AB9" s="122"/>
+      <c r="AC9" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="126"/>
-      <c r="AE9" s="126"/>
-      <c r="AF9" s="126"/>
-      <c r="AG9" s="127"/>
+      <c r="AD9" s="121"/>
+      <c r="AE9" s="121"/>
+      <c r="AF9" s="121"/>
+      <c r="AG9" s="122"/>
       <c r="AH9" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="AI9" s="126"/>
-      <c r="AJ9" s="126"/>
-      <c r="AK9" s="126"/>
-      <c r="AL9" s="127"/>
+      <c r="AI9" s="121"/>
+      <c r="AJ9" s="121"/>
+      <c r="AK9" s="121"/>
+      <c r="AL9" s="122"/>
       <c r="AM9" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="AN9" s="126"/>
-      <c r="AO9" s="126"/>
-      <c r="AP9" s="126"/>
-      <c r="AQ9" s="127"/>
+      <c r="AN9" s="121"/>
+      <c r="AO9" s="121"/>
+      <c r="AP9" s="121"/>
+      <c r="AQ9" s="122"/>
       <c r="AR9" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="AS9" s="126"/>
-      <c r="AT9" s="126"/>
-      <c r="AU9" s="126"/>
-      <c r="AV9" s="127"/>
+      <c r="AS9" s="121"/>
+      <c r="AT9" s="121"/>
+      <c r="AU9" s="121"/>
+      <c r="AV9" s="122"/>
       <c r="AW9" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="AX9" s="126"/>
-      <c r="AY9" s="126"/>
-      <c r="AZ9" s="126"/>
-      <c r="BA9" s="127"/>
-      <c r="BB9" s="128" t="s">
+      <c r="AX9" s="121"/>
+      <c r="AY9" s="121"/>
+      <c r="AZ9" s="121"/>
+      <c r="BA9" s="122"/>
+      <c r="BB9" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="BC9" s="115"/>
-      <c r="BD9" s="115"/>
-      <c r="BE9" s="115"/>
-      <c r="BF9" s="117"/>
-      <c r="BG9" s="128" t="s">
+      <c r="BC9" s="127"/>
+      <c r="BD9" s="127"/>
+      <c r="BE9" s="127"/>
+      <c r="BF9" s="128"/>
+      <c r="BG9" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="BH9" s="115"/>
-      <c r="BI9" s="115"/>
-      <c r="BJ9" s="115"/>
-      <c r="BK9" s="117"/>
-      <c r="BL9" s="128" t="s">
+      <c r="BH9" s="127"/>
+      <c r="BI9" s="127"/>
+      <c r="BJ9" s="127"/>
+      <c r="BK9" s="128"/>
+      <c r="BL9" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="BM9" s="115"/>
-      <c r="BN9" s="115"/>
-      <c r="BO9" s="115"/>
-      <c r="BP9" s="117"/>
-      <c r="BQ9" s="129" t="s">
+      <c r="BM9" s="127"/>
+      <c r="BN9" s="127"/>
+      <c r="BO9" s="127"/>
+      <c r="BP9" s="128"/>
+      <c r="BQ9" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="BR9" s="135"/>
-      <c r="BS9" s="135"/>
-      <c r="BT9" s="135"/>
-      <c r="BU9" s="136"/>
-      <c r="BV9" s="129" t="s">
+      <c r="BR9" s="119"/>
+      <c r="BS9" s="119"/>
+      <c r="BT9" s="119"/>
+      <c r="BU9" s="120"/>
+      <c r="BV9" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="BW9" s="126"/>
-      <c r="BX9" s="126"/>
-      <c r="BY9" s="126"/>
-      <c r="BZ9" s="127"/>
-      <c r="CA9" s="129" t="s">
+      <c r="BW9" s="121"/>
+      <c r="BX9" s="121"/>
+      <c r="BY9" s="121"/>
+      <c r="BZ9" s="122"/>
+      <c r="CA9" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="CB9" s="126"/>
-      <c r="CC9" s="126"/>
-      <c r="CD9" s="126"/>
-      <c r="CE9" s="127"/>
-      <c r="CF9" s="129" t="s">
+      <c r="CB9" s="121"/>
+      <c r="CC9" s="121"/>
+      <c r="CD9" s="121"/>
+      <c r="CE9" s="122"/>
+      <c r="CF9" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="CG9" s="126"/>
-      <c r="CH9" s="126"/>
-      <c r="CI9" s="126"/>
-      <c r="CJ9" s="127"/>
+      <c r="CG9" s="121"/>
+      <c r="CH9" s="121"/>
+      <c r="CI9" s="121"/>
+      <c r="CJ9" s="122"/>
     </row>
     <row r="10" spans="1:88" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="110"/>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
       <c r="I10" s="30" t="s">
         <v>29</v>
       </c>
@@ -2632,12 +2632,12 @@
     </row>
     <row r="11" spans="1:88" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
-      <c r="B11" s="110"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="113"/>
       <c r="H11" s="35" t="s">
         <v>33</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="BJ11" s="38">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="BK11" s="38">
         <v>6.5</v>
@@ -2897,134 +2897,134 @@
       <c r="H12" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="132">
+      <c r="I12" s="115">
         <f>SUM(I11:M11)</f>
         <v>12</v>
       </c>
-      <c r="J12" s="110"/>
-      <c r="K12" s="110"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="133"/>
-      <c r="N12" s="132">
+      <c r="J12" s="113"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="113"/>
+      <c r="M12" s="114"/>
+      <c r="N12" s="115">
         <f>SUM(N11:R11)</f>
         <v>10</v>
       </c>
-      <c r="O12" s="110"/>
-      <c r="P12" s="110"/>
-      <c r="Q12" s="110"/>
-      <c r="R12" s="133"/>
-      <c r="S12" s="132">
+      <c r="O12" s="113"/>
+      <c r="P12" s="113"/>
+      <c r="Q12" s="113"/>
+      <c r="R12" s="114"/>
+      <c r="S12" s="115">
         <f>SUM(S11:W11)</f>
         <v>11</v>
       </c>
-      <c r="T12" s="110"/>
-      <c r="U12" s="110"/>
-      <c r="V12" s="110"/>
-      <c r="W12" s="133"/>
-      <c r="X12" s="132">
+      <c r="T12" s="113"/>
+      <c r="U12" s="113"/>
+      <c r="V12" s="113"/>
+      <c r="W12" s="114"/>
+      <c r="X12" s="115">
         <f>SUM(X11:AB11)</f>
         <v>13</v>
       </c>
-      <c r="Y12" s="110"/>
-      <c r="Z12" s="110"/>
-      <c r="AA12" s="110"/>
-      <c r="AB12" s="133"/>
-      <c r="AC12" s="132">
+      <c r="Y12" s="113"/>
+      <c r="Z12" s="113"/>
+      <c r="AA12" s="113"/>
+      <c r="AB12" s="114"/>
+      <c r="AC12" s="115">
         <f>SUM(AC11:AG11)</f>
         <v>12</v>
       </c>
-      <c r="AD12" s="110"/>
-      <c r="AE12" s="110"/>
-      <c r="AF12" s="110"/>
-      <c r="AG12" s="133"/>
-      <c r="AH12" s="132">
+      <c r="AD12" s="113"/>
+      <c r="AE12" s="113"/>
+      <c r="AF12" s="113"/>
+      <c r="AG12" s="114"/>
+      <c r="AH12" s="115">
         <f>SUM(AH11:AL11)</f>
         <v>9</v>
       </c>
-      <c r="AI12" s="110"/>
-      <c r="AJ12" s="110"/>
-      <c r="AK12" s="110"/>
-      <c r="AL12" s="133"/>
-      <c r="AM12" s="132">
+      <c r="AI12" s="113"/>
+      <c r="AJ12" s="113"/>
+      <c r="AK12" s="113"/>
+      <c r="AL12" s="114"/>
+      <c r="AM12" s="115">
         <f>SUM(AM11:AQ11)</f>
         <v>4</v>
       </c>
-      <c r="AN12" s="110"/>
-      <c r="AO12" s="110"/>
-      <c r="AP12" s="110"/>
-      <c r="AQ12" s="133"/>
-      <c r="AR12" s="132">
+      <c r="AN12" s="113"/>
+      <c r="AO12" s="113"/>
+      <c r="AP12" s="113"/>
+      <c r="AQ12" s="114"/>
+      <c r="AR12" s="115">
         <f>SUM(AR11:AV11)</f>
         <v>10</v>
       </c>
-      <c r="AS12" s="110"/>
-      <c r="AT12" s="110"/>
-      <c r="AU12" s="110"/>
-      <c r="AV12" s="133"/>
-      <c r="AW12" s="132">
+      <c r="AS12" s="113"/>
+      <c r="AT12" s="113"/>
+      <c r="AU12" s="113"/>
+      <c r="AV12" s="114"/>
+      <c r="AW12" s="115">
         <f>SUM(AW11:BA11)</f>
         <v>10.5</v>
       </c>
-      <c r="AX12" s="110"/>
-      <c r="AY12" s="110"/>
-      <c r="AZ12" s="110"/>
-      <c r="BA12" s="133"/>
-      <c r="BB12" s="132">
+      <c r="AX12" s="113"/>
+      <c r="AY12" s="113"/>
+      <c r="AZ12" s="113"/>
+      <c r="BA12" s="114"/>
+      <c r="BB12" s="115">
         <f>SUM(BB11:BF11)</f>
         <v>2</v>
       </c>
-      <c r="BC12" s="110"/>
-      <c r="BD12" s="110"/>
-      <c r="BE12" s="110"/>
-      <c r="BF12" s="133"/>
-      <c r="BG12" s="134">
+      <c r="BC12" s="113"/>
+      <c r="BD12" s="113"/>
+      <c r="BE12" s="113"/>
+      <c r="BF12" s="114"/>
+      <c r="BG12" s="112">
         <f>SUM(BG11:BK11)</f>
-        <v>15</v>
-      </c>
-      <c r="BH12" s="110"/>
-      <c r="BI12" s="110"/>
-      <c r="BJ12" s="110"/>
-      <c r="BK12" s="133"/>
-      <c r="BL12" s="134">
+        <v>14.5</v>
+      </c>
+      <c r="BH12" s="113"/>
+      <c r="BI12" s="113"/>
+      <c r="BJ12" s="113"/>
+      <c r="BK12" s="114"/>
+      <c r="BL12" s="112">
         <f>SUM(BL11:BP11)</f>
         <v>0</v>
       </c>
-      <c r="BM12" s="110"/>
-      <c r="BN12" s="110"/>
-      <c r="BO12" s="110"/>
-      <c r="BP12" s="133"/>
-      <c r="BQ12" s="134">
+      <c r="BM12" s="113"/>
+      <c r="BN12" s="113"/>
+      <c r="BO12" s="113"/>
+      <c r="BP12" s="114"/>
+      <c r="BQ12" s="112">
         <f>SUM(BQ11:BU11)</f>
         <v>16</v>
       </c>
-      <c r="BR12" s="137"/>
-      <c r="BS12" s="137"/>
-      <c r="BT12" s="137"/>
-      <c r="BU12" s="138"/>
-      <c r="BV12" s="134">
+      <c r="BR12" s="116"/>
+      <c r="BS12" s="116"/>
+      <c r="BT12" s="116"/>
+      <c r="BU12" s="117"/>
+      <c r="BV12" s="112">
         <f>SUM(BV11:BZ11)</f>
         <v>16</v>
       </c>
-      <c r="BW12" s="110"/>
-      <c r="BX12" s="110"/>
-      <c r="BY12" s="110"/>
-      <c r="BZ12" s="133"/>
-      <c r="CA12" s="132">
+      <c r="BW12" s="113"/>
+      <c r="BX12" s="113"/>
+      <c r="BY12" s="113"/>
+      <c r="BZ12" s="114"/>
+      <c r="CA12" s="115">
         <f>SUM(CA11:CE11)</f>
         <v>16</v>
       </c>
-      <c r="CB12" s="110"/>
-      <c r="CC12" s="110"/>
-      <c r="CD12" s="110"/>
-      <c r="CE12" s="133"/>
-      <c r="CF12" s="132">
+      <c r="CB12" s="113"/>
+      <c r="CC12" s="113"/>
+      <c r="CD12" s="113"/>
+      <c r="CE12" s="114"/>
+      <c r="CF12" s="115">
         <f>SUM(CF11:CJ11)</f>
         <v>3</v>
       </c>
-      <c r="CG12" s="110"/>
-      <c r="CH12" s="110"/>
-      <c r="CI12" s="110"/>
-      <c r="CJ12" s="133"/>
+      <c r="CG12" s="113"/>
+      <c r="CH12" s="113"/>
+      <c r="CI12" s="113"/>
+      <c r="CJ12" s="114"/>
     </row>
     <row r="13" spans="1:88" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46"/>
@@ -5193,7 +5193,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D34" s="72"/>
       <c r="E34" s="72"/>
@@ -5391,7 +5391,7 @@
       <c r="B36" s="47">
         <v>45328</v>
       </c>
-      <c r="C36" s="142" t="s">
+      <c r="C36" s="111" t="s">
         <v>69</v>
       </c>
       <c r="D36" s="49" t="s">
@@ -5496,7 +5496,7 @@
       <c r="B37" s="47">
         <v>45357</v>
       </c>
-      <c r="C37" s="140" t="s">
+      <c r="C37" s="109" t="s">
         <v>70</v>
       </c>
       <c r="D37" s="83" t="s">
@@ -5601,8 +5601,8 @@
       <c r="B38" s="91">
         <v>45388</v>
       </c>
-      <c r="C38" s="141" t="s">
-        <v>75</v>
+      <c r="C38" s="110" t="s">
+        <v>73</v>
       </c>
       <c r="D38" s="92" t="s">
         <v>37</v>
@@ -5706,8 +5706,8 @@
       <c r="B39" s="47">
         <v>43226</v>
       </c>
-      <c r="C39" s="140" t="s">
-        <v>76</v>
+      <c r="C39" s="109" t="s">
+        <v>74</v>
       </c>
       <c r="D39" s="49" t="s">
         <v>37</v>
@@ -5812,7 +5812,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D40" s="72"/>
       <c r="E40" s="72"/>
@@ -5915,7 +5915,7 @@
         <v>45418</v>
       </c>
       <c r="F41" s="50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G41" s="83" t="e">
         <f t="shared" ref="G41:G44" si="7">DAYS360(E41,F41)</f>
@@ -6020,7 +6020,7 @@
         <v>45418</v>
       </c>
       <c r="F42" s="50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G42" s="83" t="e">
         <f t="shared" si="7"/>
@@ -6125,7 +6125,7 @@
         <v>45418</v>
       </c>
       <c r="F43" s="50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G43" s="83" t="e">
         <f t="shared" si="7"/>
@@ -6230,7 +6230,7 @@
         <v>45418</v>
       </c>
       <c r="F44" s="50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G44" s="83" t="e">
         <f t="shared" si="7"/>
@@ -9562,6 +9562,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="P5:AA5"/>
+    <mergeCell ref="I8:AG8"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="BQ8:CJ8"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AG2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="AH8:BP8"/>
+    <mergeCell ref="BQ9:BU9"/>
+    <mergeCell ref="BV9:BZ9"/>
+    <mergeCell ref="CA9:CE9"/>
+    <mergeCell ref="CF9:CJ9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="BL9:BP9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="BB9:BF9"/>
+    <mergeCell ref="BG9:BK9"/>
     <mergeCell ref="BV12:BZ12"/>
     <mergeCell ref="CA12:CE12"/>
     <mergeCell ref="CF12:CJ12"/>
@@ -9578,42 +9614,6 @@
     <mergeCell ref="BB12:BF12"/>
     <mergeCell ref="BG12:BK12"/>
     <mergeCell ref="BQ12:BU12"/>
-    <mergeCell ref="BQ9:BU9"/>
-    <mergeCell ref="BV9:BZ9"/>
-    <mergeCell ref="CA9:CE9"/>
-    <mergeCell ref="CF9:CJ9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="BL9:BP9"/>
-    <mergeCell ref="BQ8:CJ8"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AG2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="AH8:BP8"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="P5:AA5"/>
-    <mergeCell ref="I8:AG8"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="BB9:BF9"/>
-    <mergeCell ref="BG9:BK9"/>
   </mergeCells>
   <conditionalFormatting sqref="I45:BK80 H13:H17 H19:H80 BQ45:CE80">
     <cfRule type="colorScale" priority="3">

</xml_diff>